<commit_message>
edited excel template-added circle column
</commit_message>
<xml_diff>
--- a/public/download/template.xlsx
+++ b/public/download/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\king1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B3EB7B-650A-4F9D-8C35-20BCF0164F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEF10C13-BD3A-49AA-BCFD-4D386DB5E96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>الرقم الوظيفي</t>
   </si>
@@ -38,19 +38,22 @@
     <t>اسم الموظف</t>
   </si>
   <si>
-    <t>اسم المستشفى</t>
-  </si>
-  <si>
-    <t>اسم القسم</t>
-  </si>
-  <si>
-    <t>الدور الوظيفي</t>
-  </si>
-  <si>
     <t>رقم الجوال</t>
   </si>
   <si>
-    <t xml:space="preserve">فحص الرفع </t>
+    <t>فحص الرفع</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> المستشفى</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> الدائرة</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> القسم</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> الدور الوظيفي</t>
   </si>
 </sst>
 </file>
@@ -397,23 +400,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,24 +425,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15555</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>251548</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -447,10 +454,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>59724157</v>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>59714451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>